<commit_message>
integrate changes for main sequences, need to create code for last functions, need to connect to station cpu in order to continue
</commit_message>
<xml_diff>
--- a/Config files/Config.xlsx
+++ b/Config files/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft3940753-my.sharepoint.com/personal/emmanuel_celaya_fceo_mx/Documents/Documentos/FCEO/Plenty/scripts/HipotWalalightProject/Config files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC1048E6391F409A5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E04149-4B53-43C9-8B19-7FE9818AD6E4}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC1048E6391F409A5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21FD331-522E-4DDA-A782-30F2561DC6DF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,16 +50,16 @@
     <t>High Limit</t>
   </si>
   <si>
-    <t>Check Power</t>
-  </si>
-  <si>
-    <t>Validate Consumption</t>
-  </si>
-  <si>
-    <t>Validate Power</t>
-  </si>
-  <si>
     <t>Enable</t>
+  </si>
+  <si>
+    <t>CHECK_INTERLOCK</t>
+  </si>
+  <si>
+    <t>HIPOT_TEST</t>
+  </si>
+  <si>
+    <t>HIPOT_RESET</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E8" sqref="A6:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -484,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4">
         <v>23</v>
@@ -493,7 +493,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4">
         <v>23</v>
@@ -518,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
         <v>5</v>

</xml_diff>

<commit_message>
template standarization, file load for hipot changes
</commit_message>
<xml_diff>
--- a/Config files/Config.xlsx
+++ b/Config files/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft3940753-my.sharepoint.com/personal/emmanuel_celaya_fceo_mx/Documents/Documentos/FCEO/Plenty/scripts/HipotWalalightProject/Config files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emman\OneDrive - fceo.mx\Documentos\FCEO\Plenty\scripts\HipotWalalightProject\Config files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC1048E6391F409A5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21FD331-522E-4DDA-A782-30F2561DC6DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97F2283-63FB-421D-9209-621D99F5DE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="A6:E8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +493,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -510,7 +510,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>